<commit_message>
update to fix bad cell
</commit_message>
<xml_diff>
--- a/lwa_antpos/data/LWA-352 Antenna Status & System Configuration.xlsx
+++ b/lwa_antpos/data/LWA-352 Antenna Status & System Configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caltech.sharepoint.com/sites/ovro/projects/LWA Documents/WBS/WBS 2 - Physical Infrastructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89AD646B-58B6-4D1D-8AB9-CB3DAE275287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD9C941A-C8DC-4B1A-9C7D-B274B2E3660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="110" yWindow="790" windowWidth="22660" windowHeight="19510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4111" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4115" uniqueCount="1136">
   <si>
     <t>influx tag</t>
   </si>
@@ -2604,6 +2604,12 @@
     <t>LWA-273</t>
   </si>
   <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
     <t>LWA-274</t>
   </si>
   <si>
@@ -2623,6 +2629,12 @@
   </si>
   <si>
     <t>LWA-276</t>
+  </si>
+  <si>
+    <t>616</t>
+  </si>
+  <si>
+    <t>690</t>
   </si>
   <si>
     <t>LWA-277</t>
@@ -4571,12 +4583,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4946,8 +4958,8 @@
   <dimension ref="A1:AK370"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="R233" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="AG235" sqref="AG235:AG237"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J313" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomRight" activeCell="R373" sqref="R373"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -9604,7 +9616,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="43" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A43" s="86"/>
       <c r="B43" s="83" t="s">
         <v>197</v>
@@ -14496,7 +14508,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="87" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A87" s="86"/>
       <c r="B87" s="83" t="s">
         <v>331</v>
@@ -15014,7 +15026,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="92" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="92" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A92" s="86"/>
       <c r="B92" s="83" t="s">
         <v>345</v>
@@ -17002,7 +17014,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="110" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="110" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A110" s="86"/>
       <c r="B110" s="83" t="s">
         <v>396</v>
@@ -18428,7 +18440,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="123" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="123" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A123" s="86"/>
       <c r="B123" s="83" t="s">
         <v>432</v>
@@ -18833,7 +18845,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="127" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="127" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A127" s="86"/>
       <c r="B127" s="83" t="s">
         <v>444</v>
@@ -21376,7 +21388,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="150" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="150" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A150" s="86"/>
       <c r="B150" s="83" t="s">
         <v>513</v>
@@ -22011,7 +22023,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="156" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="156" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A156" s="86"/>
       <c r="B156" s="83" t="s">
         <v>529</v>
@@ -23739,7 +23751,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="172" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="172" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A172" s="86"/>
       <c r="B172" s="83" t="s">
         <v>573</v>
@@ -24370,7 +24382,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="178" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="178" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A178" s="86"/>
       <c r="B178" s="83" t="s">
         <v>587</v>
@@ -27024,7 +27036,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="202" spans="1:37" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="202" spans="1:37" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A202" s="86"/>
       <c r="B202" s="83" t="s">
         <v>656</v>
@@ -28998,7 +29010,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="220" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
+    <row r="220" spans="1:34" s="43" customFormat="1" ht="18" hidden="1" customHeight="1">
       <c r="A220" s="86"/>
       <c r="B220" s="83" t="s">
         <v>706</v>
@@ -30806,7 +30818,7 @@
         <v>39</v>
       </c>
       <c r="AG236" s="64">
-        <f t="shared" ref="AG236:AG237" si="0">32*(Y236-1) + (AE236/2)</f>
+        <f>32*(Y236-1) + (AE236/2)</f>
         <v>307</v>
       </c>
       <c r="AH236" s="73" t="s">
@@ -30920,7 +30932,7 @@
         <v>37</v>
       </c>
       <c r="AG237" s="64">
-        <f t="shared" si="0"/>
+        <f>32*(Y237-1) + (AE237/2)</f>
         <v>306</v>
       </c>
       <c r="AH237" s="73" t="s">
@@ -33637,8 +33649,8 @@
       <c r="J262" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K262" s="82" t="s">
-        <v>198</v>
+      <c r="K262" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L262" s="90" t="s">
         <v>804</v>
@@ -33954,8 +33966,8 @@
       <c r="J265" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K265" s="82" t="s">
-        <v>198</v>
+      <c r="K265" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L265" s="90" t="s">
         <v>814</v>
@@ -34061,8 +34073,8 @@
       <c r="J266" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K266" s="82" t="s">
-        <v>198</v>
+      <c r="K266" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L266" s="90" t="s">
         <v>817</v>
@@ -35228,11 +35240,15 @@
       <c r="J277" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K277" s="82" t="s">
-        <v>198</v>
-      </c>
-      <c r="L277" s="90"/>
-      <c r="M277" s="90"/>
+      <c r="K277" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="L277" s="90" t="s">
+        <v>849</v>
+      </c>
+      <c r="M277" s="90" t="s">
+        <v>850</v>
+      </c>
       <c r="N277" s="64"/>
       <c r="O277" s="64"/>
       <c r="P277" s="64">
@@ -35304,7 +35320,7 @@
     <row r="278" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A278" s="86"/>
       <c r="B278" s="83" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C278" s="109" t="s">
         <v>72</v>
@@ -35334,10 +35350,10 @@
         <v>74</v>
       </c>
       <c r="L278" s="90" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="M278" s="90" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="N278" s="64"/>
       <c r="O278" s="64"/>
@@ -35410,7 +35426,7 @@
     <row r="279" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A279" s="86"/>
       <c r="B279" s="83" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C279" s="109" t="s">
         <v>72</v>
@@ -35440,10 +35456,10 @@
         <v>74</v>
       </c>
       <c r="L279" s="90" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="M279" s="90" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="N279" s="64"/>
       <c r="O279" s="64"/>
@@ -35517,7 +35533,7 @@
     <row r="280" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A280" s="86"/>
       <c r="B280" s="83" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C280" s="109" t="s">
         <v>807</v>
@@ -35543,11 +35559,15 @@
       <c r="J280" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K280" s="82" t="s">
-        <v>198</v>
-      </c>
-      <c r="L280" s="90"/>
-      <c r="M280" s="90"/>
+      <c r="K280" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="L280" s="90" t="s">
+        <v>858</v>
+      </c>
+      <c r="M280" s="90" t="s">
+        <v>859</v>
+      </c>
       <c r="N280" s="64"/>
       <c r="O280" s="64"/>
       <c r="P280" s="64">
@@ -35619,7 +35639,7 @@
     <row r="281" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A281" s="86"/>
       <c r="B281" s="83" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="C281" s="109" t="s">
         <v>807</v>
@@ -35649,10 +35669,10 @@
         <v>74</v>
       </c>
       <c r="L281" s="90" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="M281" s="90" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="N281" s="64"/>
       <c r="O281" s="64"/>
@@ -35725,7 +35745,7 @@
     <row r="282" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A282" s="86"/>
       <c r="B282" s="83" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="C282" s="109" t="s">
         <v>807</v>
@@ -35754,11 +35774,11 @@
       <c r="K282" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="L282" s="115">
+      <c r="L282" s="116">
         <v>483</v>
       </c>
       <c r="M282" s="90" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="N282" s="64"/>
       <c r="O282" s="64"/>
@@ -35831,7 +35851,7 @@
     <row r="283" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A283" s="86"/>
       <c r="B283" s="83" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C283" s="109" t="s">
         <v>310</v>
@@ -35861,10 +35881,10 @@
         <v>74</v>
       </c>
       <c r="L283" s="90" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="M283" s="90" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="N283" s="64"/>
       <c r="O283" s="64"/>
@@ -35938,7 +35958,7 @@
     <row r="284" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A284" s="86"/>
       <c r="B284" s="83" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="C284" s="109" t="s">
         <v>793</v>
@@ -35968,10 +35988,10 @@
         <v>74</v>
       </c>
       <c r="L284" s="90" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="M284" s="90" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="N284" s="64"/>
       <c r="O284" s="64"/>
@@ -36044,7 +36064,7 @@
     <row r="285" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A285" s="86"/>
       <c r="B285" s="83" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="C285" s="109" t="s">
         <v>807</v>
@@ -36074,10 +36094,10 @@
         <v>74</v>
       </c>
       <c r="L285" s="90" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="M285" s="90" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="N285" s="64"/>
       <c r="O285" s="64"/>
@@ -36150,7 +36170,7 @@
     <row r="286" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A286" s="86"/>
       <c r="B286" s="83" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="C286" s="109" t="s">
         <v>807</v>
@@ -36180,10 +36200,10 @@
         <v>74</v>
       </c>
       <c r="L286" s="90" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="M286" s="90" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
       <c r="N286" s="64"/>
       <c r="O286" s="64"/>
@@ -36256,7 +36276,7 @@
     <row r="287" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A287" s="86"/>
       <c r="B287" s="83" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="C287" s="109" t="s">
         <v>793</v>
@@ -36286,10 +36306,10 @@
         <v>74</v>
       </c>
       <c r="L287" s="90" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="M287" s="90" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="N287" s="64"/>
       <c r="O287" s="64"/>
@@ -36362,7 +36382,7 @@
     <row r="288" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A288" s="86"/>
       <c r="B288" s="83" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="C288" s="109" t="s">
         <v>793</v>
@@ -36392,10 +36412,10 @@
         <v>74</v>
       </c>
       <c r="L288" s="90" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="M288" s="90" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="N288" s="64"/>
       <c r="O288" s="64"/>
@@ -36468,7 +36488,7 @@
     <row r="289" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A289" s="86"/>
       <c r="B289" s="83" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="C289" s="109" t="s">
         <v>807</v>
@@ -36498,10 +36518,10 @@
         <v>74</v>
       </c>
       <c r="L289" s="90" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
       <c r="M289" s="90" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="N289" s="64"/>
       <c r="O289" s="64"/>
@@ -36574,7 +36594,7 @@
     <row r="290" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A290" s="86"/>
       <c r="B290" s="83" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="C290" s="109" t="s">
         <v>72</v>
@@ -36604,10 +36624,10 @@
         <v>74</v>
       </c>
       <c r="L290" s="90" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="M290" s="90" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="N290" s="64"/>
       <c r="O290" s="64"/>
@@ -36681,7 +36701,7 @@
     <row r="291" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A291" s="86"/>
       <c r="B291" s="83" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="C291" s="109" t="s">
         <v>310</v>
@@ -36711,10 +36731,10 @@
         <v>74</v>
       </c>
       <c r="L291" s="90" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="M291" s="90" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="N291" s="64"/>
       <c r="O291" s="64"/>
@@ -36788,7 +36808,7 @@
     <row r="292" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A292" s="86"/>
       <c r="B292" s="83" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="C292" s="109" t="s">
         <v>793</v>
@@ -36818,10 +36838,10 @@
         <v>74</v>
       </c>
       <c r="L292" s="90" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="M292" s="90" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="N292" s="64"/>
       <c r="O292" s="64"/>
@@ -36894,7 +36914,7 @@
     <row r="293" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A293" s="86"/>
       <c r="B293" s="83" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c r="C293" s="109" t="s">
         <v>179</v>
@@ -36924,10 +36944,10 @@
         <v>74</v>
       </c>
       <c r="L293" s="90" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="M293" s="90" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="N293" s="64"/>
       <c r="O293" s="64"/>
@@ -37001,7 +37021,7 @@
     <row r="294" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A294" s="86"/>
       <c r="B294" s="83" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="C294" s="109" t="s">
         <v>475</v>
@@ -37031,10 +37051,10 @@
         <v>74</v>
       </c>
       <c r="L294" s="90" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="M294" s="90" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
       <c r="N294" s="64"/>
       <c r="O294" s="64"/>
@@ -37108,7 +37128,7 @@
     <row r="295" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A295" s="86"/>
       <c r="B295" s="83" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="C295" s="109" t="s">
         <v>793</v>
@@ -37134,14 +37154,14 @@
       <c r="J295" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K295" s="82" t="s">
-        <v>198</v>
+      <c r="K295" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L295" s="90" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c r="M295" s="90" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="N295" s="64"/>
       <c r="O295" s="64"/>
@@ -37214,7 +37234,7 @@
     <row r="296" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A296" s="86"/>
       <c r="B296" s="83" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="C296" s="109" t="s">
         <v>793</v>
@@ -37244,10 +37264,10 @@
         <v>74</v>
       </c>
       <c r="L296" s="90" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c r="M296" s="90" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="N296" s="64"/>
       <c r="O296" s="64"/>
@@ -37320,7 +37340,7 @@
     <row r="297" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A297" s="86"/>
       <c r="B297" s="83" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c r="C297" s="109" t="s">
         <v>475</v>
@@ -37350,10 +37370,10 @@
         <v>74</v>
       </c>
       <c r="L297" s="90" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="M297" s="90" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="N297" s="64"/>
       <c r="O297" s="64"/>
@@ -37427,7 +37447,7 @@
     <row r="298" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A298" s="86"/>
       <c r="B298" s="83" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="C298" s="109" t="s">
         <v>179</v>
@@ -37457,10 +37477,10 @@
         <v>74</v>
       </c>
       <c r="L298" s="90" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="M298" s="90" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="N298" s="64"/>
       <c r="O298" s="64"/>
@@ -37534,7 +37554,7 @@
     <row r="299" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A299" s="86"/>
       <c r="B299" s="83" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="C299" s="109" t="s">
         <v>793</v>
@@ -37564,10 +37584,10 @@
         <v>74</v>
       </c>
       <c r="L299" s="90" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
       <c r="M299" s="90" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="N299" s="64"/>
       <c r="O299" s="64"/>
@@ -37640,7 +37660,7 @@
     <row r="300" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A300" s="86"/>
       <c r="B300" s="83" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="C300" s="109" t="s">
         <v>793</v>
@@ -37670,10 +37690,10 @@
         <v>74</v>
       </c>
       <c r="L300" s="90" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="M300" s="90" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="N300" s="64"/>
       <c r="O300" s="64"/>
@@ -37746,7 +37766,7 @@
     <row r="301" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A301" s="86"/>
       <c r="B301" s="83" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="C301" s="109" t="s">
         <v>575</v>
@@ -37772,14 +37792,14 @@
       <c r="J301" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K301" s="82" t="s">
-        <v>198</v>
+      <c r="K301" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L301" s="90" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="M301" s="90" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="N301" s="64"/>
       <c r="O301" s="64"/>
@@ -37853,7 +37873,7 @@
     <row r="302" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A302" s="86"/>
       <c r="B302" s="83" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="C302" s="109" t="s">
         <v>793</v>
@@ -37879,14 +37899,14 @@
       <c r="J302" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K302" s="82" t="s">
-        <v>198</v>
+      <c r="K302" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L302" s="90" t="s">
         <v>829</v>
       </c>
       <c r="M302" s="90" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="N302" s="64"/>
       <c r="O302" s="64"/>
@@ -37959,7 +37979,7 @@
     <row r="303" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A303" s="86"/>
       <c r="B303" s="83" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="C303" s="109" t="s">
         <v>179</v>
@@ -37985,14 +38005,14 @@
       <c r="J303" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K303" s="82" t="s">
-        <v>198</v>
+      <c r="K303" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L303" s="90" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="M303" s="90" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="N303" s="64"/>
       <c r="O303" s="64"/>
@@ -38066,7 +38086,7 @@
     <row r="304" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A304" s="86"/>
       <c r="B304" s="83" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="C304" s="109" t="s">
         <v>592</v>
@@ -38092,14 +38112,14 @@
       <c r="J304" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K304" s="82" t="s">
-        <v>198</v>
+      <c r="K304" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L304" s="90" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="M304" s="90" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="N304" s="64"/>
       <c r="O304" s="64"/>
@@ -38173,7 +38193,7 @@
     <row r="305" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A305" s="86"/>
       <c r="B305" s="83" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="C305" s="109" t="s">
         <v>793</v>
@@ -38203,10 +38223,10 @@
         <v>74</v>
       </c>
       <c r="L305" s="90" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c r="M305" s="90" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="N305" s="64"/>
       <c r="O305" s="64"/>
@@ -38279,7 +38299,7 @@
     <row r="306" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A306" s="86"/>
       <c r="B306" s="83" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="C306" s="109" t="s">
         <v>72</v>
@@ -38309,10 +38329,10 @@
         <v>74</v>
       </c>
       <c r="L306" s="90" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="M306" s="90" t="s">
-        <v>931</v>
+        <v>935</v>
       </c>
       <c r="N306" s="64"/>
       <c r="O306" s="64"/>
@@ -38386,7 +38406,7 @@
     <row r="307" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A307" s="86"/>
       <c r="B307" s="83" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="C307" s="109" t="s">
         <v>793</v>
@@ -38416,10 +38436,10 @@
         <v>74</v>
       </c>
       <c r="L307" s="90" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="M307" s="90" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="N307" s="64"/>
       <c r="O307" s="64"/>
@@ -38492,7 +38512,7 @@
     <row r="308" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A308" s="86"/>
       <c r="B308" s="83" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="C308" s="109" t="s">
         <v>592</v>
@@ -38522,10 +38542,10 @@
         <v>74</v>
       </c>
       <c r="L308" s="90" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="M308" s="90" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="N308" s="64"/>
       <c r="O308" s="64"/>
@@ -38599,7 +38619,7 @@
     <row r="309" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A309" s="86"/>
       <c r="B309" s="83" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="C309" s="109" t="s">
         <v>793</v>
@@ -38629,10 +38649,10 @@
         <v>74</v>
       </c>
       <c r="L309" s="90" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="M309" s="90" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="N309" s="64"/>
       <c r="O309" s="64"/>
@@ -38705,7 +38725,7 @@
     <row r="310" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A310" s="86"/>
       <c r="B310" s="83" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="C310" s="109" t="s">
         <v>793</v>
@@ -38735,10 +38755,10 @@
         <v>74</v>
       </c>
       <c r="L310" s="90" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="M310" s="90" t="s">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c r="N310" s="64"/>
       <c r="O310" s="64"/>
@@ -38811,7 +38831,7 @@
     <row r="311" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A311" s="86"/>
       <c r="B311" s="83" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="C311" s="109" t="s">
         <v>807</v>
@@ -38841,10 +38861,10 @@
         <v>74</v>
       </c>
       <c r="L311" s="90" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="M311" s="90" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="N311" s="64"/>
       <c r="O311" s="64"/>
@@ -38917,7 +38937,7 @@
     <row r="312" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A312" s="86"/>
       <c r="B312" s="83" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="C312" s="109" t="s">
         <v>807</v>
@@ -38947,10 +38967,10 @@
         <v>74</v>
       </c>
       <c r="L312" s="90" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="M312" s="90" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="N312" s="64"/>
       <c r="O312" s="64"/>
@@ -39023,7 +39043,7 @@
     <row r="313" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A313" s="86"/>
       <c r="B313" s="83" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="C313" s="109" t="s">
         <v>807</v>
@@ -39053,10 +39073,10 @@
         <v>74</v>
       </c>
       <c r="L313" s="90" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="M313" s="90" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="N313" s="64"/>
       <c r="O313" s="64"/>
@@ -39129,7 +39149,7 @@
     <row r="314" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A314" s="86"/>
       <c r="B314" s="83" t="s">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c r="C314" s="109" t="s">
         <v>807</v>
@@ -39159,10 +39179,10 @@
         <v>74</v>
       </c>
       <c r="L314" s="90" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
       <c r="M314" s="90" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="N314" s="64"/>
       <c r="O314" s="64"/>
@@ -39235,7 +39255,7 @@
     <row r="315" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A315" s="86"/>
       <c r="B315" s="83" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="C315" s="109" t="s">
         <v>807</v>
@@ -39265,10 +39285,10 @@
         <v>74</v>
       </c>
       <c r="L315" s="90" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="M315" s="90" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="N315" s="64"/>
       <c r="O315" s="64"/>
@@ -39341,7 +39361,7 @@
     <row r="316" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A316" s="86"/>
       <c r="B316" s="83" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C316" s="109" t="s">
         <v>807</v>
@@ -39371,10 +39391,10 @@
         <v>74</v>
       </c>
       <c r="L316" s="90" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="M316" s="90" t="s">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c r="N316" s="64"/>
       <c r="O316" s="64"/>
@@ -39447,7 +39467,7 @@
     <row r="317" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A317" s="86"/>
       <c r="B317" s="83" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="C317" s="109" t="s">
         <v>807</v>
@@ -39477,7 +39497,7 @@
         <v>74</v>
       </c>
       <c r="L317" s="90" t="s">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c r="M317" s="90" t="s">
         <v>736</v>
@@ -39553,7 +39573,7 @@
     <row r="318" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A318" s="86"/>
       <c r="B318" s="83" t="s">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="C318" s="109" t="s">
         <v>807</v>
@@ -39583,10 +39603,10 @@
         <v>74</v>
       </c>
       <c r="L318" s="90" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="M318" s="90" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="N318" s="64"/>
       <c r="O318" s="64"/>
@@ -39659,7 +39679,7 @@
     <row r="319" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A319" s="86"/>
       <c r="B319" s="83" t="s">
-        <v>967</v>
+        <v>971</v>
       </c>
       <c r="C319" s="109" t="s">
         <v>592</v>
@@ -39689,10 +39709,10 @@
         <v>74</v>
       </c>
       <c r="L319" s="90" t="s">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c r="M319" s="90" t="s">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c r="N319" s="64"/>
       <c r="O319" s="64"/>
@@ -39766,7 +39786,7 @@
     <row r="320" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A320" s="86"/>
       <c r="B320" s="83" t="s">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c r="C320" s="109" t="s">
         <v>163</v>
@@ -39796,10 +39816,10 @@
         <v>74</v>
       </c>
       <c r="L320" s="90" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c r="M320" s="90" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="N320" s="64"/>
       <c r="O320" s="64"/>
@@ -39873,7 +39893,7 @@
     <row r="321" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A321" s="86"/>
       <c r="B321" s="83" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="C321" s="109" t="s">
         <v>793</v>
@@ -39903,10 +39923,10 @@
         <v>74</v>
       </c>
       <c r="L321" s="90" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="M321" s="90" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="N321" s="64"/>
       <c r="O321" s="64"/>
@@ -39979,7 +39999,7 @@
     <row r="322" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A322" s="86"/>
       <c r="B322" s="83" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="C322" s="109" t="s">
         <v>793</v>
@@ -40009,10 +40029,10 @@
         <v>74</v>
       </c>
       <c r="L322" s="90" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="M322" s="90" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="N322" s="64"/>
       <c r="O322" s="64"/>
@@ -40085,7 +40105,7 @@
     <row r="323" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A323" s="86"/>
       <c r="B323" s="83" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="C323" s="109" t="s">
         <v>179</v>
@@ -40111,14 +40131,14 @@
       <c r="J323" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K323" s="82" t="s">
-        <v>198</v>
+      <c r="K323" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L323" s="90" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="M323" s="90" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="N323" s="64"/>
       <c r="O323" s="64"/>
@@ -40192,7 +40212,7 @@
     <row r="324" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A324" s="86"/>
       <c r="B324" s="83" t="s">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c r="C324" s="109" t="s">
         <v>793</v>
@@ -40222,10 +40242,10 @@
         <v>74</v>
       </c>
       <c r="L324" s="90" t="s">
-        <v>982</v>
+        <v>986</v>
       </c>
       <c r="M324" s="90" t="s">
-        <v>983</v>
+        <v>987</v>
       </c>
       <c r="N324" s="64"/>
       <c r="O324" s="64"/>
@@ -40298,7 +40318,7 @@
     <row r="325" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A325" s="86"/>
       <c r="B325" s="83" t="s">
-        <v>984</v>
+        <v>988</v>
       </c>
       <c r="C325" s="109" t="s">
         <v>807</v>
@@ -40328,10 +40348,10 @@
         <v>74</v>
       </c>
       <c r="L325" s="90" t="s">
-        <v>985</v>
+        <v>989</v>
       </c>
       <c r="M325" s="90" t="s">
-        <v>986</v>
+        <v>990</v>
       </c>
       <c r="N325" s="64"/>
       <c r="O325" s="64"/>
@@ -40404,7 +40424,7 @@
     <row r="326" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A326" s="86"/>
       <c r="B326" s="83" t="s">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>446</v>
@@ -40434,7 +40454,7 @@
         <v>74</v>
       </c>
       <c r="L326" s="90" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="M326" s="90" t="s">
         <v>770</v>
@@ -40511,7 +40531,7 @@
     <row r="327" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A327" s="86"/>
       <c r="B327" s="83" t="s">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>72</v>
@@ -40541,10 +40561,10 @@
         <v>74</v>
       </c>
       <c r="L327" s="90" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="M327" s="90" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="N327" s="64"/>
       <c r="O327" s="64"/>
@@ -40618,7 +40638,7 @@
     <row r="328" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A328" s="86"/>
       <c r="B328" s="83" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>116</v>
@@ -40721,7 +40741,7 @@
     <row r="329" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A329" s="86"/>
       <c r="B329" s="83" t="s">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>163</v>
@@ -40751,10 +40771,10 @@
         <v>74</v>
       </c>
       <c r="L329" s="90" t="s">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c r="M329" s="90" t="s">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c r="N329" s="64"/>
       <c r="O329" s="64"/>
@@ -40828,7 +40848,7 @@
     <row r="330" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A330" s="86"/>
       <c r="B330" s="83" t="s">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>446</v>
@@ -40858,10 +40878,10 @@
         <v>74</v>
       </c>
       <c r="L330" s="90" t="s">
-        <v>996</v>
+        <v>1000</v>
       </c>
       <c r="M330" s="90" t="s">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c r="N330" s="64"/>
       <c r="O330" s="64"/>
@@ -40935,7 +40955,7 @@
     <row r="331" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A331" s="86"/>
       <c r="B331" s="83" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>807</v>
@@ -40965,10 +40985,10 @@
         <v>74</v>
       </c>
       <c r="L331" s="90" t="s">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c r="M331" s="90" t="s">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c r="N331" s="64"/>
       <c r="O331" s="64"/>
@@ -41041,7 +41061,7 @@
     <row r="332" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A332" s="86"/>
       <c r="B332" s="83" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>163</v>
@@ -41071,10 +41091,10 @@
         <v>74</v>
       </c>
       <c r="L332" s="90" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="M332" s="90" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="N332" s="64"/>
       <c r="O332" s="64"/>
@@ -41148,7 +41168,7 @@
     <row r="333" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A333" s="86"/>
       <c r="B333" s="83" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>475</v>
@@ -41178,10 +41198,10 @@
         <v>74</v>
       </c>
       <c r="L333" s="90" t="s">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="M333" s="90" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="N333" s="64"/>
       <c r="O333" s="64"/>
@@ -41255,7 +41275,7 @@
     <row r="334" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A334" s="86"/>
       <c r="B334" s="83" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>807</v>
@@ -41285,10 +41305,10 @@
         <v>74</v>
       </c>
       <c r="L334" s="90" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="M334" s="90" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="N334" s="64"/>
       <c r="O334" s="64"/>
@@ -41361,7 +41381,7 @@
     <row r="335" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A335" s="86"/>
       <c r="B335" s="83" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>116</v>
@@ -41391,10 +41411,10 @@
         <v>74</v>
       </c>
       <c r="L335" s="90" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="M335" s="90" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="N335" s="64"/>
       <c r="O335" s="64"/>
@@ -41468,7 +41488,7 @@
     <row r="336" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A336" s="86"/>
       <c r="B336" s="83" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>807</v>
@@ -41498,10 +41518,10 @@
         <v>74</v>
       </c>
       <c r="L336" s="90" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="M336" s="90" t="s">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="N336" s="64"/>
       <c r="O336" s="64"/>
@@ -41574,7 +41594,7 @@
     <row r="337" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A337" s="86"/>
       <c r="B337" s="83" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>446</v>
@@ -41681,7 +41701,7 @@
     <row r="338" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A338" s="86"/>
       <c r="B338" s="83" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>163</v>
@@ -41711,10 +41731,10 @@
         <v>74</v>
       </c>
       <c r="L338" s="90" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="M338" s="90" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="N338" s="64"/>
       <c r="O338" s="64"/>
@@ -41788,7 +41808,7 @@
     <row r="339" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A339" s="86"/>
       <c r="B339" s="83" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>793</v>
@@ -41818,10 +41838,10 @@
         <v>74</v>
       </c>
       <c r="L339" s="90" t="s">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="M339" s="90" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="N339" s="64"/>
       <c r="O339" s="64"/>
@@ -41894,7 +41914,7 @@
     <row r="340" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A340" s="86"/>
       <c r="B340" s="83" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>793</v>
@@ -41924,10 +41944,10 @@
         <v>74</v>
       </c>
       <c r="L340" s="90" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="M340" s="90" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="N340" s="64"/>
       <c r="O340" s="64"/>
@@ -42000,7 +42020,7 @@
     <row r="341" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A341" s="86"/>
       <c r="B341" s="83" t="s">
-        <v>1024</v>
+        <v>1028</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>793</v>
@@ -42030,10 +42050,10 @@
         <v>74</v>
       </c>
       <c r="L341" s="90" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="M341" s="90" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="N341" s="64"/>
       <c r="O341" s="64"/>
@@ -42106,7 +42126,7 @@
     <row r="342" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A342" s="86"/>
       <c r="B342" s="83" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>807</v>
@@ -42136,10 +42156,10 @@
         <v>74</v>
       </c>
       <c r="L342" s="90" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="M342" s="90" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="N342" s="64"/>
       <c r="O342" s="64"/>
@@ -42212,7 +42232,7 @@
     <row r="343" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A343" s="86"/>
       <c r="B343" s="83" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>807</v>
@@ -42242,10 +42262,10 @@
         <v>74</v>
       </c>
       <c r="L343" s="90" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="M343" s="90" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="N343" s="64"/>
       <c r="O343" s="64"/>
@@ -42318,7 +42338,7 @@
     <row r="344" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A344" s="86"/>
       <c r="B344" s="83" t="s">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>807</v>
@@ -42348,10 +42368,10 @@
         <v>74</v>
       </c>
       <c r="L344" s="90" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="M344" s="90" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="N344" s="64"/>
       <c r="O344" s="64"/>
@@ -42424,7 +42444,7 @@
     <row r="345" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A345" s="86"/>
       <c r="B345" s="83" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>807</v>
@@ -42454,10 +42474,10 @@
         <v>74</v>
       </c>
       <c r="L345" s="90" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c r="M345" s="90" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
       <c r="N345" s="64"/>
       <c r="O345" s="64"/>
@@ -42530,7 +42550,7 @@
     <row r="346" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A346" s="86"/>
       <c r="B346" s="83" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>575</v>
@@ -42560,10 +42580,10 @@
         <v>74</v>
       </c>
       <c r="L346" s="90" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="M346" s="90" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="N346" s="64"/>
       <c r="O346" s="64"/>
@@ -42637,7 +42657,7 @@
     <row r="347" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A347" s="86"/>
       <c r="B347" s="83" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>793</v>
@@ -42667,10 +42687,10 @@
         <v>74</v>
       </c>
       <c r="L347" s="90" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="M347" s="90" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
       <c r="N347" s="64"/>
       <c r="O347" s="64"/>
@@ -42743,7 +42763,7 @@
     <row r="348" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A348" s="86"/>
       <c r="B348" s="83" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>793</v>
@@ -42769,14 +42789,14 @@
       <c r="J348" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K348" s="82" t="s">
-        <v>198</v>
+      <c r="K348" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L348" s="90" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="M348" s="90" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
       <c r="N348" s="64"/>
       <c r="O348" s="64"/>
@@ -42849,7 +42869,7 @@
     <row r="349" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A349" s="86"/>
       <c r="B349" s="83" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>446</v>
@@ -42879,10 +42899,10 @@
         <v>74</v>
       </c>
       <c r="L349" s="90" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="M349" s="90" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
       <c r="N349" s="64"/>
       <c r="O349" s="64"/>
@@ -42956,7 +42976,7 @@
     <row r="350" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A350" s="86"/>
       <c r="B350" s="83" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>575</v>
@@ -42986,10 +43006,10 @@
         <v>74</v>
       </c>
       <c r="L350" s="90" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="M350" s="90" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
       <c r="N350" s="64"/>
       <c r="O350" s="64"/>
@@ -43063,7 +43083,7 @@
     <row r="351" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A351" s="86"/>
       <c r="B351" s="83" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>446</v>
@@ -43093,10 +43113,10 @@
         <v>74</v>
       </c>
       <c r="L351" s="90" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="M351" s="90" t="s">
-        <v>1054</v>
+        <v>1058</v>
       </c>
       <c r="N351" s="64"/>
       <c r="O351" s="64"/>
@@ -43170,7 +43190,7 @@
     <row r="352" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A352" s="86"/>
       <c r="B352" s="83" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>116</v>
@@ -43200,10 +43220,10 @@
         <v>74</v>
       </c>
       <c r="L352" s="90" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="M352" s="90" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
       <c r="N352" s="64"/>
       <c r="O352" s="64"/>
@@ -43277,7 +43297,7 @@
     <row r="353" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A353" s="86"/>
       <c r="B353" s="83" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>475</v>
@@ -43307,10 +43327,10 @@
         <v>74</v>
       </c>
       <c r="L353" s="90" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c r="M353" s="90" t="s">
-        <v>1060</v>
+        <v>1064</v>
       </c>
       <c r="N353" s="64"/>
       <c r="O353" s="64"/>
@@ -43383,7 +43403,7 @@
     <row r="354" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A354" s="86"/>
       <c r="B354" s="83" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>575</v>
@@ -43413,10 +43433,10 @@
         <v>74</v>
       </c>
       <c r="L354" s="90" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="M354" s="90" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="N354" s="64"/>
       <c r="O354" s="64"/>
@@ -43490,7 +43510,7 @@
     <row r="355" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A355" s="86"/>
       <c r="B355" s="83" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>793</v>
@@ -43516,14 +43536,14 @@
       <c r="J355" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="K355" s="82" t="s">
-        <v>198</v>
+      <c r="K355" s="81" t="s">
+        <v>74</v>
       </c>
       <c r="L355" s="90" t="s">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c r="M355" s="90" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="N355" s="64"/>
       <c r="O355" s="64"/>
@@ -43596,7 +43616,7 @@
     <row r="356" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A356" s="86"/>
       <c r="B356" s="83" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>807</v>
@@ -43626,10 +43646,10 @@
         <v>74</v>
       </c>
       <c r="L356" s="90" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="M356" s="90" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="N356" s="64"/>
       <c r="O356" s="64"/>
@@ -43702,7 +43722,7 @@
     <row r="357" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A357" s="86"/>
       <c r="B357" s="83" t="s">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>807</v>
@@ -43732,10 +43752,10 @@
         <v>74</v>
       </c>
       <c r="L357" s="90" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="M357" s="90" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
       <c r="N357" s="64"/>
       <c r="O357" s="64"/>
@@ -43808,7 +43828,7 @@
     <row r="358" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A358" s="86"/>
       <c r="B358" s="83" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>793</v>
@@ -43838,10 +43858,10 @@
         <v>74</v>
       </c>
       <c r="L358" s="90" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="M358" s="90" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
       <c r="N358" s="64"/>
       <c r="O358" s="64"/>
@@ -43914,7 +43934,7 @@
     <row r="359" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A359" s="86"/>
       <c r="B359" s="83" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>310</v>
@@ -43944,10 +43964,10 @@
         <v>74</v>
       </c>
       <c r="L359" s="90" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c r="M359" s="90" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
       <c r="N359" s="64"/>
       <c r="O359" s="64"/>
@@ -44021,7 +44041,7 @@
     <row r="360" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A360" s="86"/>
       <c r="B360" s="83" t="s">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>575</v>
@@ -44051,10 +44071,10 @@
         <v>74</v>
       </c>
       <c r="L360" s="90" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="M360" s="90" t="s">
-        <v>1079</v>
+        <v>1083</v>
       </c>
       <c r="N360" s="64"/>
       <c r="O360" s="64"/>
@@ -44128,7 +44148,7 @@
     <row r="361" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A361" s="86"/>
       <c r="B361" s="83" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>475</v>
@@ -44161,7 +44181,7 @@
         <v>399</v>
       </c>
       <c r="M361" s="90" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="N361" s="64"/>
       <c r="O361" s="64"/>
@@ -44235,7 +44255,7 @@
     <row r="362" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A362" s="86"/>
       <c r="B362" s="83" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>163</v>
@@ -44265,10 +44285,10 @@
         <v>74</v>
       </c>
       <c r="L362" s="90" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="M362" s="90" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="N362" s="64"/>
       <c r="O362" s="64"/>
@@ -44342,7 +44362,7 @@
     <row r="363" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A363" s="86"/>
       <c r="B363" s="83" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>446</v>
@@ -44372,10 +44392,10 @@
         <v>74</v>
       </c>
       <c r="L363" s="90" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c r="M363" s="90" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
       <c r="N363" s="64"/>
       <c r="O363" s="64"/>
@@ -44386,20 +44406,22 @@
         <f>_xlfn.XLOOKUP(P363,'ARX IDs'!B$3:B$47,'ARX IDs'!C$3:C$47,"")</f>
         <v>4110</v>
       </c>
-      <c r="R363" s="64"/>
+      <c r="R363" s="64">
+        <v>12</v>
+      </c>
       <c r="S363" s="64">
         <v>11</v>
       </c>
       <c r="T363" s="80">
         <f>100 * $R363 + S363</f>
-        <v>11</v>
+        <v>1211</v>
       </c>
       <c r="U363" s="77">
         <v>12</v>
       </c>
       <c r="V363" s="80">
         <f>100 * $R363 + U363</f>
-        <v>12</v>
+        <v>1212</v>
       </c>
       <c r="W363" s="64">
         <f>IF(ISBLANK(Y363), "", _xlfn.XLOOKUP(Y363,'SNAP2 IDs'!C$3:C$15,'SNAP2 IDs'!B$3:B$15,""))</f>
@@ -44446,7 +44468,7 @@
     <row r="364" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A364" s="86"/>
       <c r="B364" s="83" t="s">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>793</v>
@@ -44476,10 +44498,10 @@
         <v>74</v>
       </c>
       <c r="L364" s="90" t="s">
-        <v>1088</v>
+        <v>1092</v>
       </c>
       <c r="M364" s="90" t="s">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c r="N364" s="64"/>
       <c r="O364" s="64"/>
@@ -44552,7 +44574,7 @@
     <row r="365" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A365" s="86"/>
       <c r="B365" s="83" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>163</v>
@@ -44582,10 +44604,10 @@
         <v>74</v>
       </c>
       <c r="L365" s="90" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
       <c r="M365" s="90" t="s">
-        <v>1092</v>
+        <v>1096</v>
       </c>
       <c r="N365" s="64"/>
       <c r="O365" s="64"/>
@@ -44659,7 +44681,7 @@
     <row r="366" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A366" s="86"/>
       <c r="B366" s="83" t="s">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>807</v>
@@ -44689,10 +44711,10 @@
         <v>74</v>
       </c>
       <c r="L366" s="90" t="s">
-        <v>1094</v>
+        <v>1098</v>
       </c>
       <c r="M366" s="90" t="s">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c r="N366" s="64"/>
       <c r="O366" s="64"/>
@@ -44765,7 +44787,7 @@
     <row r="367" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A367" s="86"/>
       <c r="B367" s="83" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>72</v>
@@ -44795,10 +44817,10 @@
         <v>74</v>
       </c>
       <c r="L367" s="90" t="s">
-        <v>1097</v>
+        <v>1101</v>
       </c>
       <c r="M367" s="90" t="s">
-        <v>1098</v>
+        <v>1102</v>
       </c>
       <c r="N367" s="64"/>
       <c r="O367" s="64"/>
@@ -44872,7 +44894,7 @@
     <row r="368" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A368" s="86"/>
       <c r="B368" s="83" t="s">
-        <v>1099</v>
+        <v>1103</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>116</v>
@@ -44902,10 +44924,10 @@
         <v>74</v>
       </c>
       <c r="L368" s="90" t="s">
-        <v>1100</v>
+        <v>1104</v>
       </c>
       <c r="M368" s="90" t="s">
-        <v>1101</v>
+        <v>1105</v>
       </c>
       <c r="N368" s="64"/>
       <c r="O368" s="64"/>
@@ -44979,7 +45001,7 @@
     <row r="369" spans="1:34" s="43" customFormat="1" ht="18" customHeight="1">
       <c r="A369" s="86"/>
       <c r="B369" s="84" t="s">
-        <v>1102</v>
+        <v>1106</v>
       </c>
       <c r="C369" s="109" t="s">
         <v>116</v>
@@ -45030,7 +45052,7 @@
         <f>100 * $R369 + S369</f>
         <v>1005</v>
       </c>
-      <c r="U369" s="116">
+      <c r="U369" s="115">
         <v>6</v>
       </c>
       <c r="V369" s="80">
@@ -45078,13 +45100,13 @@
         <v>126</v>
       </c>
       <c r="AH369" s="74" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="370" spans="1:34" ht="18.75" customHeight="1">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="370" spans="1:34" ht="18.75" hidden="1" customHeight="1">
       <c r="A370" s="86"/>
       <c r="B370" s="85" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="C370" s="109"/>
       <c r="D370" s="71" t="s">
@@ -45115,7 +45137,7 @@
         <v>457</v>
       </c>
       <c r="M370" s="90" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="N370" s="64"/>
       <c r="O370" s="64"/>
@@ -45150,7 +45172,7 @@
       <c r="AF370" s="64"/>
       <c r="AG370" s="64"/>
       <c r="AH370" s="75" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
     </row>
   </sheetData>
@@ -45208,25 +45230,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="94" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="B1" s="100" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="C1" s="100" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="D1" s="103" t="s">
-        <v>1110</v>
+        <v>1114</v>
       </c>
       <c r="E1" s="96" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
       <c r="F1" s="95" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="G1" s="95" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -65707,7 +65729,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>1114</v>
+        <v>1118</v>
       </c>
       <c r="F3" s="36" t="str">
         <f t="shared" ref="F3:F15" si="1">IF(ISBLANK(C3), "", CONCATENATE(IF(C3 &lt; 10, "snap0", "snap"),C3,".sas.pvt"))</f>
@@ -65747,7 +65769,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>1115</v>
+        <v>1119</v>
       </c>
       <c r="F5" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65767,7 +65789,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="F6" s="36" t="str">
         <f>IF(ISBLANK(C6), "", CONCATENATE(IF(C6 &lt; 10, "snap0", "snap"),C6,".sas.pvt"))</f>
@@ -65787,7 +65809,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c r="F7" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65807,7 +65829,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
       <c r="F8" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65827,7 +65849,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c r="F9" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65847,7 +65869,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>1120</v>
+        <v>1124</v>
       </c>
       <c r="F10" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65883,7 +65905,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="F12" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65919,7 +65941,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1122</v>
+        <v>1126</v>
       </c>
       <c r="F14" s="36" t="str">
         <f t="shared" si="1"/>
@@ -65939,7 +65961,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>1123</v>
+        <v>1127</v>
       </c>
       <c r="F15" s="63" t="str">
         <f t="shared" si="1"/>
@@ -65969,7 +65991,7 @@
   <dimension ref="B1:C47"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="C11" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -66382,7 +66404,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="29" t="s">
-        <v>1124</v>
+        <v>1128</v>
       </c>
       <c r="C2" s="29"/>
     </row>
@@ -66391,7 +66413,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>1125</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="33" customFormat="1" ht="35.25" customHeight="1">
@@ -66399,7 +66421,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>1126</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="6" spans="2:4" s="33" customFormat="1" ht="35.25" customHeight="1">
@@ -66407,7 +66429,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>1127</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="7" spans="2:4" s="33" customFormat="1">
@@ -66415,7 +66437,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>1128</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="33" customFormat="1" ht="53.25" customHeight="1">
@@ -66423,7 +66445,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>1129</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="33" customFormat="1" ht="66" customHeight="1">
@@ -66431,7 +66453,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>1130</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="33" customFormat="1" ht="29.1">
@@ -66439,7 +66461,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>1131</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="11" spans="2:4" s="33" customFormat="1">
@@ -66679,17 +66701,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100969A852156D25941A1952AB04D85E27D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbd588d986b09d3cd3368ebef1dc2ddf">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2c70659-2d8e-48dd-af6d-da2141f5031a" xmlns:ns3="56c45531-4dc0-4ecf-b1f6-b3e259fe0aa2" xmlns:ns4="70f2d024-d81a-45b9-9f62-d57c478f1068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed33987256813058b290e6f461af9725" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100969A852156D25941A1952AB04D85E27D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f7847a3ba26feda94cd0562e7482524">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2c70659-2d8e-48dd-af6d-da2141f5031a" xmlns:ns3="56c45531-4dc0-4ecf-b1f6-b3e259fe0aa2" xmlns:ns4="70f2d024-d81a-45b9-9f62-d57c478f1068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e18765d3cf247826546bf8b9eca620c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="a2c70659-2d8e-48dd-af6d-da2141f5031a"/>
     <xsd:import namespace="56c45531-4dc0-4ecf-b1f6-b3e259fe0aa2"/>
     <xsd:import namespace="70f2d024-d81a-45b9-9f62-d57c478f1068"/>
@@ -66715,6 +66728,7 @@
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:_Flow_SignoffStatus" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -66794,6 +66808,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="24" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Flow_SignoffStatus" ma:index="25" nillable="true" ma:displayName="Sign-off status" ma:internalName="Sign_x002d_off_x0020_status">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -66941,6 +66960,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -66948,16 +66976,17 @@
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <_Flow_SignoffStatus xmlns="a2c70659-2d8e-48dd-af6d-da2141f5031a" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3F821CB-369E-4104-A49A-9E03773B151F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F132938E-50EB-496E-B02A-4296A2795E42}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74473091-30BF-4BDB-BA41-129CD76ED00F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3F821CB-369E-4104-A49A-9E03773B151F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>